<commit_message>
D-Scores unit tests (in development)
</commit_message>
<xml_diff>
--- a/framework_demos/meta/tests_dscores.scores.iat.xlsx
+++ b/framework_demos/meta/tests_dscores.scores.iat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>set_id</t>
   </si>
@@ -96,13 +96,16 @@
   </si>
   <si>
     <t>too_fast</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,16 +121,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,14 +172,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,12 +481,13 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:Q1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -491,35 +547,391 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>375</v>
+      </c>
+      <c r="H2" s="3">
+        <v>64.54972243679029</v>
+      </c>
+      <c r="I2">
+        <f>G2+H2*2</f>
+        <v>504.09944487358058</v>
+      </c>
+      <c r="J2">
+        <v>375</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>425</v>
+      </c>
+      <c r="M2" s="3">
+        <v>64.54972243679029</v>
+      </c>
+      <c r="N2">
+        <f>L2+M2*2</f>
+        <v>554.09944487358052</v>
+      </c>
+      <c r="O2">
+        <v>425</v>
+      </c>
+      <c r="P2" s="5">
+        <v>65.465367070797711</v>
+      </c>
+      <c r="Q2">
+        <f>(O2-J2)/P2</f>
+        <v>0.76376261582597338</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>450</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3">
+        <v>450</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>475</v>
+      </c>
+      <c r="M3" s="9">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N4" si="0">L3+M3*2</f>
+        <v>545.71067811865476</v>
+      </c>
+      <c r="O3">
+        <v>475</v>
+      </c>
+      <c r="P3" s="6">
+        <v>28.867513459480953</v>
+      </c>
+      <c r="Q3">
+        <f>(O3-J3)/P3</f>
+        <v>0.8660254037844487</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4" s="7">
+        <v>70.710678118654755</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I3:I4" si="1">G4+H4*2</f>
+        <v>541.42135623730951</v>
+      </c>
+      <c r="J4" s="10">
+        <v>470.71067811865476</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>425</v>
+      </c>
+      <c r="M4" s="8">
+        <v>64.54972243679029</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>554.09944487358052</v>
+      </c>
+      <c r="O4">
+        <v>425</v>
+      </c>
+      <c r="P4" s="11">
+        <v>77.163029811779168</v>
+      </c>
+      <c r="Q4">
+        <f>(O4-J4)/P4</f>
+        <v>-0.59239091868418159</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>400</v>
+      </c>
+      <c r="H5">
+        <v>50</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I8" si="2">G5+H5*2</f>
+        <v>500</v>
+      </c>
+      <c r="J5">
+        <v>400</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>425</v>
+      </c>
+      <c r="M5" s="6">
+        <v>64.54972243679029</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N8" si="3">L5+M5*2</f>
+        <v>554.09944487358052</v>
+      </c>
+      <c r="O5">
+        <v>425</v>
+      </c>
+      <c r="P5" s="4">
+        <v>55.634864026418782</v>
+      </c>
+      <c r="Q5">
+        <f>(O5-J5)/P5</f>
+        <v>0.44935851713645775</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>400</v>
+      </c>
+      <c r="H6" s="6">
+        <v>70.710678118654755</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>541.42135623730951</v>
+      </c>
+      <c r="J6" s="6">
+        <v>400</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>425</v>
+      </c>
+      <c r="M6" s="6">
+        <v>64.54972243679029</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>554.09944487358052</v>
+      </c>
+      <c r="O6">
+        <v>425</v>
+      </c>
+      <c r="P6" s="4">
+        <v>60.553007081949893</v>
+      </c>
+      <c r="Q6">
+        <f>(O6-J6)/P6</f>
+        <v>0.41286141192238485</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>144</v>
+      </c>
+      <c r="C7">
+        <v>137</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>71</v>
+      </c>
+      <c r="G7" s="6">
+        <v>675.91549295774644</v>
+      </c>
+      <c r="H7" s="6">
+        <v>191.81425140550297</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1059.5439957687524</v>
+      </c>
+      <c r="J7" s="6">
+        <v>681.24366661111117</v>
+      </c>
+      <c r="K7">
+        <v>66</v>
+      </c>
+      <c r="L7" s="6">
+        <v>854.89393939393938</v>
+      </c>
+      <c r="M7" s="6">
+        <v>261.77430847600112</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>1378.4425563459417</v>
+      </c>
+      <c r="O7" s="6">
+        <v>871.94811077777786</v>
+      </c>
+      <c r="P7" s="4">
+        <v>246.85994800247437</v>
+      </c>
+      <c r="Q7">
+        <f>(O7-J7)/P7</f>
+        <v>0.77252079857342915</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <v>83</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1025.625</v>
+      </c>
+      <c r="H8" s="6">
+        <v>271.50461886405566</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1568.6342377281112</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1294.5106507042253</v>
+      </c>
+      <c r="K8">
+        <v>51</v>
+      </c>
+      <c r="L8" s="6">
+        <v>993.64705882352939</v>
+      </c>
+      <c r="M8" s="6">
+        <v>241.9671732718644</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>1477.5814053672582</v>
+      </c>
+      <c r="O8" s="6">
+        <v>1134.7945764583335</v>
+      </c>
+      <c r="P8" s="4">
+        <v>286.06111226276363</v>
+      </c>
+      <c r="Q8">
+        <f>(O8-J8)/P8</f>
+        <v>-0.55832850883689289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted the scores manually calculated for the d-score unit tests
</commit_message>
<xml_diff>
--- a/framework_demos/meta/tests_dscores.scores.iat.xlsx
+++ b/framework_demos/meta/tests_dscores.scores.iat.xlsx
@@ -481,7 +481,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
         <v>65.465367070797711</v>
       </c>
       <c r="Q2">
-        <f>(O2-J2)/P2</f>
+        <f t="shared" ref="Q2:Q8" si="0">(O2-J2)/P2</f>
         <v>0.76376261582597338</v>
       </c>
     </row>
@@ -640,7 +640,7 @@
         <v>35.355339059327378</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N4" si="0">L3+M3*2</f>
+        <f t="shared" ref="N3:N4" si="1">L3+M3*2</f>
         <v>545.71067811865476</v>
       </c>
       <c r="O3">
@@ -650,7 +650,7 @@
         <v>28.867513459480953</v>
       </c>
       <c r="Q3">
-        <f>(O3-J3)/P3</f>
+        <f t="shared" si="0"/>
         <v>0.8660254037844487</v>
       </c>
     </row>
@@ -680,7 +680,7 @@
         <v>70.710678118654755</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I3:I4" si="1">G4+H4*2</f>
+        <f t="shared" ref="I4" si="2">G4+H4*2</f>
         <v>541.42135623730951</v>
       </c>
       <c r="J4" s="10">
@@ -696,7 +696,7 @@
         <v>64.54972243679029</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>554.09944487358052</v>
       </c>
       <c r="O4">
@@ -706,7 +706,7 @@
         <v>77.163029811779168</v>
       </c>
       <c r="Q4">
-        <f>(O4-J4)/P4</f>
+        <f t="shared" si="0"/>
         <v>-0.59239091868418159</v>
       </c>
     </row>
@@ -736,7 +736,7 @@
         <v>50</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I8" si="2">G5+H5*2</f>
+        <f t="shared" ref="I5:I8" si="3">G5+H5*2</f>
         <v>500</v>
       </c>
       <c r="J5">
@@ -752,7 +752,7 @@
         <v>64.54972243679029</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N8" si="3">L5+M5*2</f>
+        <f t="shared" ref="N5:N8" si="4">L5+M5*2</f>
         <v>554.09944487358052</v>
       </c>
       <c r="O5">
@@ -762,7 +762,7 @@
         <v>55.634864026418782</v>
       </c>
       <c r="Q5">
-        <f>(O5-J5)/P5</f>
+        <f t="shared" si="0"/>
         <v>0.44935851713645775</v>
       </c>
     </row>
@@ -792,7 +792,7 @@
         <v>70.710678118654755</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>541.42135623730951</v>
       </c>
       <c r="J6" s="6">
@@ -808,7 +808,7 @@
         <v>64.54972243679029</v>
       </c>
       <c r="N6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>554.09944487358052</v>
       </c>
       <c r="O6">
@@ -818,7 +818,7 @@
         <v>60.553007081949893</v>
       </c>
       <c r="Q6">
-        <f>(O6-J6)/P6</f>
+        <f t="shared" si="0"/>
         <v>0.41286141192238485</v>
       </c>
     </row>
@@ -848,7 +848,7 @@
         <v>191.81425140550297</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1059.5439957687524</v>
       </c>
       <c r="J7" s="6">
@@ -864,18 +864,18 @@
         <v>261.77430847600112</v>
       </c>
       <c r="N7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1378.4425563459417</v>
       </c>
       <c r="O7" s="6">
-        <v>871.94811077777786</v>
-      </c>
-      <c r="P7" s="4">
-        <v>246.85994800247437</v>
+        <v>862.70809789999998</v>
+      </c>
+      <c r="P7" s="6">
+        <v>249.45765120005558</v>
       </c>
       <c r="Q7">
-        <f>(O7-J7)/P7</f>
-        <v>0.77252079857342915</v>
+        <f t="shared" si="0"/>
+        <v>0.72743582093363501</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -895,20 +895,20 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="6">
-        <v>1025.625</v>
+        <v>1058.2903225806451</v>
       </c>
       <c r="H8" s="6">
-        <v>271.50461886405566</v>
+        <v>202.21031848851314</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
-        <v>1568.6342377281112</v>
+        <f t="shared" si="3"/>
+        <v>1462.7109595576715</v>
       </c>
       <c r="J8" s="6">
-        <v>1294.5106507042253</v>
+        <v>1281.0147315942022</v>
       </c>
       <c r="K8">
         <v>51</v>
@@ -920,18 +920,18 @@
         <v>241.9671732718644</v>
       </c>
       <c r="N8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1477.5814053672582</v>
       </c>
       <c r="O8" s="6">
         <v>1134.7945764583335</v>
       </c>
-      <c r="P8" s="4">
-        <v>286.06111226276363</v>
+      <c r="P8" s="6">
+        <v>282.63187952757147</v>
       </c>
       <c r="Q8">
-        <f>(O8-J8)/P8</f>
-        <v>-0.55832850883689289</v>
+        <f t="shared" si="0"/>
+        <v>-0.51735195399853873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>